<commit_message>
cambie el path de opcion 5
</commit_message>
<xml_diff>
--- a/Empleados.xlsx
+++ b/Empleados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arman\Documents\doc_uach\segundo_semestre\introduccion_a_la_programacion\parcial_3\ProP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4999822-9877-4B44-B82E-2598F4DF94C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95749E6F-7FF5-4592-B0EA-39329966B48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,6 +864,8 @@
       <c r="F3" s="1">
         <v>3</v>
       </c>
+      <c r="G3"/>
+      <c r="H3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -964,6 +966,8 @@
       <c r="F8" s="1">
         <v>3</v>
       </c>
+      <c r="G8"/>
+      <c r="H8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1104,6 +1108,8 @@
       <c r="F15" s="1">
         <v>3</v>
       </c>
+      <c r="G15"/>
+      <c r="H15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1125,7 +1131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1144,8 +1150,10 @@
       <c r="F17" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17"/>
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1165,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1185,7 +1193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1205,7 +1213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1225,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -1245,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1265,7 +1273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -1285,7 +1293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -1305,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -1325,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -1345,7 +1353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -1364,8 +1372,10 @@
       <c r="F28" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -1385,7 +1395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>94</v>
       </c>
@@ -1405,7 +1415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -1424,8 +1434,10 @@
       <c r="F31" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31"/>
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -1444,8 +1456,10 @@
       <c r="F32" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32"/>
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -1464,8 +1478,10 @@
       <c r="F33" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33"/>
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -1485,7 +1501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -1505,7 +1521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>112</v>
       </c>
@@ -1525,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -1545,7 +1561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>118</v>
       </c>
@@ -1564,8 +1580,10 @@
       <c r="F38" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38"/>
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>121</v>
       </c>
@@ -1584,8 +1602,10 @@
       <c r="F39" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39"/>
+      <c r="H39"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>124</v>
       </c>
@@ -1604,8 +1624,10 @@
       <c r="F40" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40"/>
+      <c r="H40"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
Se arreglo la funcion de retardos
</commit_message>
<xml_diff>
--- a/Empleados.xlsx
+++ b/Empleados.xlsx
@@ -460,8 +460,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -988,7 +988,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">

</xml_diff>

<commit_message>
No hice nada basicamente
</commit_message>
<xml_diff>
--- a/Empleados.xlsx
+++ b/Empleados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="9960" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="EMPLEADOS" sheetId="1" state="visible" r:id="rId1"/>
@@ -447,13 +447,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="16.44140625" customWidth="1" min="2" max="2"/>
     <col width="24.5546875" customWidth="1" min="3" max="3"/>
@@ -970,7 +970,7 @@
       </c>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>I</t>
         </is>
       </c>
       <c r="E18" s="1" t="n">
@@ -1622,6 +1622,33 @@
       </c>
       <c r="F41" s="1" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="42"/>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>999999</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Probado</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>